<commit_message>
Femto release data update - MPD
</commit_message>
<xml_diff>
--- a/Femto_자료 전달 List.xlsx
+++ b/Femto_자료 전달 List.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8449A9C-96CA-475D-8CFD-9D13627CBC66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23145" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Pipette" sheetId="1" r:id="rId1"/>
+    <sheet name="MPD" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t>Pipette</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,62 +86,174 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>전달 Data List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원본 설계 자료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V5.0 Issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery 오동작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간헐적으로 Power off 후 전원이 안켜짐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery 탈부착 or charger 탈부착 후 정상 동작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Off 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD는 정상 동작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Pipette_V2.1_0.5sec_2,3,4msec.bin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Pipette_V2.1_0.5sec_3,4,5msec.bin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Pipette_V2.1_1.0sec_2,3,4msec.bin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Pipette_V2.1_1.0sec_3,4,5msec.bin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>재요청에 의해 재송부</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>전달 Data List</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>원본 설계 자료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구분</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Model</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Comment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V5.0 Issue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Battery 오동작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>간헐적으로 Power off 후 전원이 안켜짐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Battery 탈부착 or charger 탈부착 후 정상 동작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Plasma Off 안됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MPD는 정상 동작</t>
+    <t>Plasma On time 수정 요청에 의한 F/W release</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD-MAIN_SCH_V1.0_20190807.sch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD-MAIN_SCH_V1.0_20190807.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD-MAIN_PCB_V1.0_20190807_Gerber.zip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD-MAIN_PCB_V1.0_20190807.pcb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD MAIN PCB PL V1.0_20190807.xlsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD-LED_SCH_V1.0_20190807.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD-LED_SCH_V1.0_20190807.sch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD-LED_PCB_V1.0_20190807_Gerber.zip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD-LED_PCB_V1.0_20190807.pcb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD LED_PCB PL_V1.0_20190807.xlsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KEY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD-KEY_SCH_V1.0_20190807.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD-KEY_SCH_V1.0_20190807.sch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD-KEY_PCB_V1.0_20190807_Gerber.zip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD-KEY_PCB_V1.0_20190807.pcb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD-KEY_PCB PL V1.0_20190807.xlsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plasma_pt.zip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD SW_V1.0.bin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPD V1.0 수정 사항_20190922.xlsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정 사항</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -209,16 +320,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -230,9 +338,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -293,7 +406,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,26 +439,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -378,23 +474,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -570,148 +649,224 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C5:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="50.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:8" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="5" t="s">
+    <row r="5" spans="3:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="8">
         <v>43922</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
       <c r="E7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="7"/>
     </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="7"/>
+      <c r="D14" s="8">
+        <v>43926</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D26" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="C6:C17"/>
+    <mergeCell ref="H14:H17"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C6:C13"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D6:D13"/>
     <mergeCell ref="H6:H13"/>
@@ -723,65 +878,253 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B4:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="8">
+        <v>43927</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B4:B15"/>
+    <mergeCell ref="C4:C15"/>
+    <mergeCell ref="G4:G15"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D10:D12"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>